<commit_message>
Added Comm. Protocol for Ass2
</commit_message>
<xml_diff>
--- a/Documents/SENG696 Architecture.xlsx
+++ b/Documents/SENG696 Architecture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ispar\Desktop\SENG696_Repo\SENG696\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ispar\Desktop\SENG696\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590DE04B-00D0-4AF8-A1E2-2E142F6E1561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EC8919-BC3A-4F85-B003-91EEEB266A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{C6A042E6-D3C1-40DC-ACFB-48C7EC627BF5}"/>
+    <workbookView xWindow="3288" yWindow="2412" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="5" xr2:uid="{C6A042E6-D3C1-40DC-ACFB-48C7EC627BF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Role Model" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Agent Model" sheetId="3" r:id="rId3"/>
     <sheet name="Service Model" sheetId="4" r:id="rId4"/>
     <sheet name="Acquaintance Model" sheetId="5" r:id="rId5"/>
+    <sheet name="Comm. Protocol" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
   <si>
     <t>Role Schema</t>
   </si>
@@ -258,13 +259,124 @@
   </si>
   <si>
     <t>CSV file exists</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>SendLabeledImage</t>
+  </si>
+  <si>
+    <t>SendStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent </t>
+  </si>
+  <si>
+    <t>IA Agent</t>
+  </si>
+  <si>
+    <t>IP Agent</t>
+  </si>
+  <si>
+    <t>FV Agent</t>
+  </si>
+  <si>
+    <t>DB Agent</t>
+  </si>
+  <si>
+    <t>Error Code</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Command Format</t>
+  </si>
+  <si>
+    <t>Sender Agent ID</t>
+  </si>
+  <si>
+    <t>Receiver Agent ID</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>1Char</t>
+  </si>
+  <si>
+    <t>X Char</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>RequestLabelledImage</t>
+  </si>
+  <si>
+    <t>"1"</t>
+  </si>
+  <si>
+    <t>"3"</t>
+  </si>
+  <si>
+    <t>"0"</t>
+  </si>
+  <si>
+    <t>"FileName"</t>
+  </si>
+  <si>
+    <t>"2"</t>
+  </si>
+  <si>
+    <t>"File_String"</t>
+  </si>
+  <si>
+    <t>"Classification:Accuracy"</t>
+  </si>
+  <si>
+    <t>Image Report</t>
+  </si>
+  <si>
+    <t>Requesting DB Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reporting file type</t>
+  </si>
+  <si>
+    <t>Requesting image processing</t>
+  </si>
+  <si>
+    <t>Checking file for image</t>
+  </si>
+  <si>
+    <t>"4"</t>
+  </si>
+  <si>
+    <t>Acknowledge data storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0" or "1" </t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>0=True,  1=False</t>
+  </si>
+  <si>
+    <t>Accuracy Format- XXX.XX%</t>
+  </si>
+  <si>
+    <t>0=Success, 1=Failure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,8 +384,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +418,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -518,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -620,20 +758,61 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -754,6 +933,20 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E732718-2A6F-49C9-B863-AB8BEB53549D}" name="Table2" displayName="Table2" ref="B14:G26" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0">
+  <tableColumns count="6">
+    <tableColumn id="8" xr3:uid="{DD076011-BB26-4C00-A9E1-EBCC240E6252}" name="Command" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A2FD8B63-CF08-43F5-B9D8-4BA296BC2206}" name="Sender Agent ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{5031E6C3-3ECC-497C-BEDE-AAD512B4379B}" name="Receiver Agent ID" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{B070F534-FA43-423C-82FD-07886C71DADE}" name="Error Code" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{75B68A7C-3A46-49CF-AD78-7091C6F926CC}" name="Data" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{77D053A1-4DB1-4FB2-80B2-DF8F39B795B0}" name="Description" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1070,10 +1263,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1117,7 +1310,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
@@ -1127,10 +1320,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1367,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
@@ -1184,10 +1377,10 @@
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1231,7 +1424,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="37"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="19" t="s">
         <v>11</v>
       </c>
@@ -1241,10 +1434,10 @@
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="36"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1288,7 +1481,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="37"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="19" t="s">
         <v>11</v>
       </c>
@@ -1298,14 +1491,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -1318,6 +1503,14 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1561,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE9B7B7-4E0E-4C9C-AF8E-5D95878F939C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
@@ -1570,4 +1763,336 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F202BC01-EDFA-4D1C-8660-DD4FC4EB9F37}">
+  <dimension ref="B2:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="41">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="41">
+        <v>2</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="41">
+        <v>3</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="41">
+        <v>4</v>
+      </c>
+      <c r="F6" s="41"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="38"/>
+      <c r="C8" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Handled exceptions and final integration
</commit_message>
<xml_diff>
--- a/Documents/SENG696 Architecture.xlsx
+++ b/Documents/SENG696 Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ispar\Desktop\SENG696\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6F8A75-8191-4422-8108-3E358AF99C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298199C8-A4D9-43A1-963C-E7B5D42C6E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{C6A042E6-D3C1-40DC-ACFB-48C7EC627BF5}"/>
   </bookViews>
@@ -325,9 +325,6 @@
     <t>"0"</t>
   </si>
   <si>
-    <t>"FileName"</t>
-  </si>
-  <si>
     <t>"2"</t>
   </si>
   <si>
@@ -374,6 +371,9 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>" "</t>
   </si>
 </sst>
 </file>
@@ -781,13 +781,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1484,10 +1484,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
@@ -1541,10 +1541,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="42"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1588,7 +1588,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
@@ -1598,10 +1598,10 @@
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="42"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1645,7 +1645,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="40"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="19" t="s">
         <v>11</v>
       </c>
@@ -1655,10 +1655,10 @@
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="40"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="19" t="s">
         <v>11</v>
       </c>
@@ -1712,6 +1712,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -1724,14 +1732,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1993,8 +1993,8 @@
   </sheetPr>
   <dimension ref="B2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2048,7 +2048,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" s="12">
         <v>1</v>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -2166,10 +2166,10 @@
         <v>91</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -2191,13 +2191,13 @@
         <v>89</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -2216,16 +2216,16 @@
         <v>89</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>91</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -2241,19 +2241,19 @@
         <v>72</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>89</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F22" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -2263,7 +2263,7 @@
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -2274,16 +2274,16 @@
         <v>89</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>91</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -2293,7 +2293,7 @@
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -2301,19 +2301,19 @@
         <v>73</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>89</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Final code cleaning and organisation
</commit_message>
<xml_diff>
--- a/Documents/SENG696 Architecture.xlsx
+++ b/Documents/SENG696 Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ispar\Desktop\SENG696\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298199C8-A4D9-43A1-963C-E7B5D42C6E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7529A332-432D-4CBE-B76F-A2440113D2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{C6A042E6-D3C1-40DC-ACFB-48C7EC627BF5}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="115">
   <si>
     <t>Role Schema</t>
   </si>
@@ -373,7 +373,25 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>" "</t>
+    <t>FileDecodeError</t>
+  </si>
+  <si>
+    <t>DatabaseNotFound</t>
+  </si>
+  <si>
+    <t>FileEncodeError</t>
+  </si>
+  <si>
+    <t>"File_Name "</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0", "1" or "2" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0", "3" or "4" </t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1175,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E732718-2A6F-49C9-B863-AB8BEB53549D}" name="Table2" displayName="Table2" ref="B15:G27" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E732718-2A6F-49C9-B863-AB8BEB53549D}" name="Table2" displayName="Table2" ref="B16:G28" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="6">
     <tableColumn id="8" xr3:uid="{DD076011-BB26-4C00-A9E1-EBCC240E6252}" name="Command" dataDxfId="5"/>
     <tableColumn id="1" xr3:uid="{A2FD8B63-CF08-43F5-B9D8-4BA296BC2206}" name="Sender Agent ID" dataDxfId="4"/>
@@ -1991,10 +2009,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:G27"/>
+  <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2061,8 +2079,12 @@
       <c r="C5" s="36">
         <v>3</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
@@ -2071,263 +2093,280 @@
       <c r="C6" s="36">
         <v>4</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="36"/>
+      <c r="F7" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="33"/>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="34"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="33"/>
+      <c r="C9" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D10" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E10" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F10" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="36" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D11" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E11" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F11" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="44" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
       <c r="F13" s="45"/>
       <c r="G13" s="45"/>
     </row>
-    <row r="15" spans="2:7" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="12" t="s">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+    </row>
+    <row r="16" spans="2:7" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D16" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G16" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="12" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C17" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D17" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E17" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="G16" s="12" t="s">
+      <c r="F17" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D19" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G19" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="12" t="s">
+      <c r="E23" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G23" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="12" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D25" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F25" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G25" s="12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="12" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D27" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="12" t="s">
+      <c r="E27" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G27" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="B12:G13"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="portrait" r:id="rId1"/>
@@ -2341,7 +2380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358557BE-8DAE-432D-A9D3-E534BBE2D000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>

</xml_diff>